<commit_message>
worked on student admin
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data.xlsx
+++ b/src/main/resources/UMS_Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="24">
   <si>
     <t>Subject Code</t>
   </si>
@@ -645,6 +645,12 @@
   </si>
   <si>
     <t>ss</t>
+  </si>
+  <si>
+    <t>thera thmith</t>
+  </si>
+  <si>
+    <t>0.4</t>
   </si>
 </sst>
 </file>
@@ -6303,7 +6309,7 @@
         <v>71</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>208</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>73</v>
@@ -6329,8 +6335,8 @@
       <c r="J2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="10">
-        <v>0.40000000000000002</v>
+      <c r="K2" s="10" t="s">
+        <v>209</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
fixed student managment after gui update
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data.xlsx
+++ b/src/main/resources/UMS_Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="24">
   <si>
     <t>Subject Code</t>
   </si>
@@ -6309,7 +6309,7 @@
         <v>71</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>208</v>
+        <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>73</v>

</xml_diff>